<commit_message>
Central fed. dist. 11-12 (added) & RO corr.
</commit_message>
<xml_diff>
--- a/migforecasting/cities11-12/0/d1.xlsx
+++ b/migforecasting/cities11-12/0/d1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="947">
   <si>
     <t>Ростов-на-Дону</t>
   </si>
@@ -1150,74 +1150,6 @@
   </si>
   <si>
     <t>5,9</t>
-  </si>
-  <si>
-    <t>Численность детей, стоящих на учете 
-для определения в дошкольные образо-
-вательные организации, человек</t>
-  </si>
-  <si>
-    <t>5179</t>
-  </si>
-  <si>
-    <t>10335</t>
-  </si>
-  <si>
-    <t>25533</t>
-  </si>
-  <si>
-    <t>1759</t>
-  </si>
-  <si>
-    <t>3179</t>
-  </si>
-  <si>
-    <t>3633</t>
-  </si>
-  <si>
-    <t>806</t>
-  </si>
-  <si>
-    <t>4087</t>
-  </si>
-  <si>
-    <t>4105</t>
-  </si>
-  <si>
-    <t>4698</t>
-  </si>
-  <si>
-    <t>3453</t>
-  </si>
-  <si>
-    <t>4654</t>
-  </si>
-  <si>
-    <t>1007</t>
-  </si>
-  <si>
-    <t>1261</t>
-  </si>
-  <si>
-    <t>1271</t>
-  </si>
-  <si>
-    <t>1626</t>
-  </si>
-  <si>
-    <t>1845</t>
-  </si>
-  <si>
-    <t>7856</t>
-  </si>
-  <si>
-    <t>1512</t>
-  </si>
-  <si>
-    <t>1688</t>
-  </si>
-  <si>
-    <t>1533</t>
   </si>
   <si>
     <t>Численность врачей, человек:</t>
@@ -2978,6 +2910,8 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3324,8 +3258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="L67" sqref="L67"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q67" sqref="Q67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5068,76 +5002,76 @@
       <c r="B28" t="s">
         <v>375</v>
       </c>
-      <c r="C28" t="s">
-        <v>376</v>
-      </c>
-      <c r="D28" t="s">
-        <v>377</v>
-      </c>
-      <c r="E28" t="s">
-        <v>378</v>
-      </c>
-      <c r="F28" t="s">
-        <v>379</v>
-      </c>
-      <c r="G28" t="s">
-        <v>380</v>
-      </c>
-      <c r="H28" t="s">
-        <v>381</v>
-      </c>
-      <c r="I28" t="s">
-        <v>382</v>
-      </c>
-      <c r="J28" t="s">
-        <v>383</v>
-      </c>
-      <c r="K28" t="s">
-        <v>384</v>
-      </c>
-      <c r="L28" t="s">
-        <v>385</v>
-      </c>
-      <c r="M28" t="s">
-        <v>386</v>
-      </c>
-      <c r="N28" t="s">
-        <v>387</v>
-      </c>
-      <c r="O28" t="s">
-        <v>388</v>
-      </c>
-      <c r="P28" t="s">
-        <v>389</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>390</v>
-      </c>
-      <c r="R28" t="s">
-        <v>391</v>
-      </c>
-      <c r="S28" t="s">
-        <v>392</v>
-      </c>
-      <c r="T28" t="s">
-        <v>393</v>
-      </c>
-      <c r="U28" t="s">
-        <v>394</v>
-      </c>
-      <c r="V28" t="s">
-        <v>395</v>
-      </c>
-      <c r="W28" t="s">
-        <v>396</v>
-      </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>397</v>
+        <v>376</v>
+      </c>
+      <c r="C29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D29" t="s">
+        <v>378</v>
+      </c>
+      <c r="E29" t="s">
+        <v>379</v>
+      </c>
+      <c r="F29" t="s">
+        <v>380</v>
+      </c>
+      <c r="G29" t="s">
+        <v>381</v>
+      </c>
+      <c r="H29" t="s">
+        <v>382</v>
+      </c>
+      <c r="I29" t="s">
+        <v>383</v>
+      </c>
+      <c r="J29" t="s">
+        <v>384</v>
+      </c>
+      <c r="K29" t="s">
+        <v>385</v>
+      </c>
+      <c r="L29" t="s">
+        <v>383</v>
+      </c>
+      <c r="M29" t="s">
+        <v>386</v>
+      </c>
+      <c r="N29" t="s">
+        <v>387</v>
+      </c>
+      <c r="O29" t="s">
+        <v>388</v>
+      </c>
+      <c r="P29" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>390</v>
+      </c>
+      <c r="R29" t="s">
+        <v>391</v>
+      </c>
+      <c r="S29" t="s">
+        <v>392</v>
+      </c>
+      <c r="T29" t="s">
+        <v>391</v>
+      </c>
+      <c r="U29" t="s">
+        <v>393</v>
+      </c>
+      <c r="V29" t="s">
+        <v>394</v>
+      </c>
+      <c r="W29" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
@@ -5145,70 +5079,70 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>396</v>
+      </c>
+      <c r="C30" t="s">
+        <v>397</v>
+      </c>
+      <c r="D30" t="s">
         <v>398</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
         <v>399</v>
       </c>
-      <c r="D30" t="s">
+      <c r="F30" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" t="s">
         <v>400</v>
       </c>
-      <c r="E30" t="s">
+      <c r="I30" t="s">
         <v>401</v>
       </c>
-      <c r="F30" t="s">
+      <c r="J30" t="s">
         <v>402</v>
       </c>
-      <c r="G30" t="s">
+      <c r="K30" t="s">
         <v>403</v>
       </c>
-      <c r="H30" t="s">
+      <c r="L30" t="s">
         <v>404</v>
       </c>
-      <c r="I30" t="s">
+      <c r="M30" t="s">
+        <v>344</v>
+      </c>
+      <c r="N30" t="s">
         <v>405</v>
       </c>
-      <c r="J30" t="s">
+      <c r="O30" t="s">
         <v>406</v>
       </c>
-      <c r="K30" t="s">
+      <c r="P30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q30" t="s">
         <v>407</v>
       </c>
-      <c r="L30" t="s">
-        <v>405</v>
-      </c>
-      <c r="M30" t="s">
+      <c r="R30" t="s">
         <v>408</v>
       </c>
-      <c r="N30" t="s">
+      <c r="S30" t="s">
         <v>409</v>
       </c>
-      <c r="O30" t="s">
+      <c r="T30" t="s">
         <v>410</v>
       </c>
-      <c r="P30" t="s">
+      <c r="U30" t="s">
         <v>411</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="V30" t="s">
+        <v>107</v>
+      </c>
+      <c r="W30" t="s">
         <v>412</v>
-      </c>
-      <c r="R30" t="s">
-        <v>413</v>
-      </c>
-      <c r="S30" t="s">
-        <v>414</v>
-      </c>
-      <c r="T30" t="s">
-        <v>413</v>
-      </c>
-      <c r="U30" t="s">
-        <v>415</v>
-      </c>
-      <c r="V30" t="s">
-        <v>416</v>
-      </c>
-      <c r="W30" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
@@ -5216,70 +5150,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>418</v>
-      </c>
-      <c r="C31" t="s">
-        <v>419</v>
-      </c>
-      <c r="D31" t="s">
-        <v>420</v>
-      </c>
-      <c r="E31" t="s">
-        <v>421</v>
-      </c>
-      <c r="F31" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" t="s">
-        <v>52</v>
-      </c>
-      <c r="H31" t="s">
-        <v>422</v>
-      </c>
-      <c r="I31" t="s">
-        <v>423</v>
-      </c>
-      <c r="J31" t="s">
-        <v>424</v>
-      </c>
-      <c r="K31" t="s">
-        <v>425</v>
-      </c>
-      <c r="L31" t="s">
-        <v>426</v>
-      </c>
-      <c r="M31" t="s">
-        <v>344</v>
-      </c>
-      <c r="N31" t="s">
-        <v>427</v>
-      </c>
-      <c r="O31" t="s">
-        <v>428</v>
-      </c>
-      <c r="P31" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>429</v>
-      </c>
-      <c r="R31" t="s">
-        <v>430</v>
-      </c>
-      <c r="S31" t="s">
-        <v>431</v>
-      </c>
-      <c r="T31" t="s">
-        <v>432</v>
-      </c>
-      <c r="U31" t="s">
-        <v>433</v>
-      </c>
-      <c r="V31" t="s">
-        <v>107</v>
-      </c>
-      <c r="W31" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
@@ -5287,7 +5158,70 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>435</v>
+        <v>376</v>
+      </c>
+      <c r="C32" t="s">
+        <v>414</v>
+      </c>
+      <c r="D32" t="s">
+        <v>415</v>
+      </c>
+      <c r="E32" t="s">
+        <v>416</v>
+      </c>
+      <c r="F32" t="s">
+        <v>417</v>
+      </c>
+      <c r="G32" t="s">
+        <v>417</v>
+      </c>
+      <c r="H32" t="s">
+        <v>418</v>
+      </c>
+      <c r="I32" t="s">
+        <v>419</v>
+      </c>
+      <c r="J32" t="s">
+        <v>420</v>
+      </c>
+      <c r="K32" t="s">
+        <v>421</v>
+      </c>
+      <c r="L32" t="s">
+        <v>422</v>
+      </c>
+      <c r="M32" t="s">
+        <v>423</v>
+      </c>
+      <c r="N32" t="s">
+        <v>424</v>
+      </c>
+      <c r="O32" t="s">
+        <v>417</v>
+      </c>
+      <c r="P32" t="s">
+        <v>425</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>426</v>
+      </c>
+      <c r="R32" t="s">
+        <v>427</v>
+      </c>
+      <c r="S32" t="s">
+        <v>428</v>
+      </c>
+      <c r="T32" t="s">
+        <v>429</v>
+      </c>
+      <c r="U32" t="s">
+        <v>430</v>
+      </c>
+      <c r="V32" t="s">
+        <v>431</v>
+      </c>
+      <c r="W32" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -5295,70 +5229,70 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C33" t="s">
+        <v>433</v>
+      </c>
+      <c r="D33" t="s">
+        <v>434</v>
+      </c>
+      <c r="E33" t="s">
+        <v>435</v>
+      </c>
+      <c r="F33" t="s">
         <v>436</v>
       </c>
-      <c r="D33" t="s">
+      <c r="G33" t="s">
         <v>437</v>
       </c>
-      <c r="E33" t="s">
+      <c r="H33" t="s">
         <v>438</v>
       </c>
-      <c r="F33" t="s">
+      <c r="I33" t="s">
         <v>439</v>
       </c>
-      <c r="G33" t="s">
-        <v>439</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="J33" t="s">
         <v>440</v>
       </c>
-      <c r="I33" t="s">
+      <c r="K33" t="s">
         <v>441</v>
       </c>
-      <c r="J33" t="s">
+      <c r="L33" t="s">
         <v>442</v>
       </c>
-      <c r="K33" t="s">
+      <c r="M33" t="s">
         <v>443</v>
       </c>
-      <c r="L33" t="s">
+      <c r="N33" t="s">
         <v>444</v>
       </c>
-      <c r="M33" t="s">
+      <c r="O33" t="s">
         <v>445</v>
       </c>
-      <c r="N33" t="s">
+      <c r="P33" t="s">
         <v>446</v>
       </c>
-      <c r="O33" t="s">
-        <v>439</v>
-      </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>447</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="R33" t="s">
         <v>448</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>449</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>450</v>
       </c>
-      <c r="T33" t="s">
+      <c r="U33" t="s">
         <v>451</v>
       </c>
-      <c r="U33" t="s">
+      <c r="V33" t="s">
         <v>452</v>
       </c>
-      <c r="V33" t="s">
+      <c r="W33" t="s">
         <v>453</v>
-      </c>
-      <c r="W33" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -5366,70 +5300,70 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>418</v>
+        <v>454</v>
       </c>
       <c r="C34" t="s">
+        <v>341</v>
+      </c>
+      <c r="D34" t="s">
+        <v>341</v>
+      </c>
+      <c r="E34" t="s">
+        <v>341</v>
+      </c>
+      <c r="F34" t="s">
         <v>455</v>
       </c>
-      <c r="D34" t="s">
+      <c r="G34" t="s">
+        <v>455</v>
+      </c>
+      <c r="H34" t="s">
+        <v>455</v>
+      </c>
+      <c r="I34" t="s">
         <v>456</v>
       </c>
-      <c r="E34" t="s">
+      <c r="J34" t="s">
+        <v>456</v>
+      </c>
+      <c r="K34" t="s">
+        <v>456</v>
+      </c>
+      <c r="L34" t="s">
         <v>457</v>
       </c>
-      <c r="F34" t="s">
+      <c r="M34" t="s">
+        <v>457</v>
+      </c>
+      <c r="N34" t="s">
         <v>458</v>
       </c>
-      <c r="G34" t="s">
+      <c r="O34" t="s">
         <v>459</v>
       </c>
-      <c r="H34" t="s">
+      <c r="P34" t="s">
+        <v>459</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>459</v>
+      </c>
+      <c r="R34" t="s">
+        <v>458</v>
+      </c>
+      <c r="S34" t="s">
+        <v>458</v>
+      </c>
+      <c r="T34" t="s">
         <v>460</v>
       </c>
-      <c r="I34" t="s">
-        <v>461</v>
-      </c>
-      <c r="J34" t="s">
-        <v>462</v>
-      </c>
-      <c r="K34" t="s">
-        <v>463</v>
-      </c>
-      <c r="L34" t="s">
-        <v>464</v>
-      </c>
-      <c r="M34" t="s">
-        <v>465</v>
-      </c>
-      <c r="N34" t="s">
-        <v>466</v>
-      </c>
-      <c r="O34" t="s">
-        <v>467</v>
-      </c>
-      <c r="P34" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>469</v>
-      </c>
-      <c r="R34" t="s">
-        <v>470</v>
-      </c>
-      <c r="S34" t="s">
-        <v>471</v>
-      </c>
-      <c r="T34" t="s">
-        <v>472</v>
-      </c>
       <c r="U34" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
       <c r="V34" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
       <c r="W34" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
@@ -5437,70 +5371,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>476</v>
-      </c>
-      <c r="C35" t="s">
-        <v>341</v>
-      </c>
-      <c r="D35" t="s">
-        <v>341</v>
-      </c>
-      <c r="E35" t="s">
-        <v>341</v>
-      </c>
-      <c r="F35" t="s">
-        <v>477</v>
-      </c>
-      <c r="G35" t="s">
-        <v>477</v>
-      </c>
-      <c r="H35" t="s">
-        <v>477</v>
-      </c>
-      <c r="I35" t="s">
-        <v>478</v>
-      </c>
-      <c r="J35" t="s">
-        <v>478</v>
-      </c>
-      <c r="K35" t="s">
-        <v>478</v>
-      </c>
-      <c r="L35" t="s">
-        <v>479</v>
-      </c>
-      <c r="M35" t="s">
-        <v>479</v>
-      </c>
-      <c r="N35" t="s">
-        <v>480</v>
-      </c>
-      <c r="O35" t="s">
-        <v>481</v>
-      </c>
-      <c r="P35" t="s">
-        <v>481</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>481</v>
-      </c>
-      <c r="R35" t="s">
-        <v>480</v>
-      </c>
-      <c r="S35" t="s">
-        <v>480</v>
-      </c>
-      <c r="T35" t="s">
-        <v>482</v>
-      </c>
-      <c r="U35" t="s">
-        <v>480</v>
-      </c>
-      <c r="V35" t="s">
-        <v>480</v>
-      </c>
-      <c r="W35" t="s">
-        <v>482</v>
+        <v>461</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
@@ -5508,7 +5379,70 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>483</v>
+        <v>462</v>
+      </c>
+      <c r="C36" t="s">
+        <v>463</v>
+      </c>
+      <c r="D36" t="s">
+        <v>464</v>
+      </c>
+      <c r="E36" t="s">
+        <v>465</v>
+      </c>
+      <c r="F36" t="s">
+        <v>466</v>
+      </c>
+      <c r="G36" t="s">
+        <v>466</v>
+      </c>
+      <c r="H36" t="s">
+        <v>467</v>
+      </c>
+      <c r="I36" t="s">
+        <v>468</v>
+      </c>
+      <c r="J36" t="s">
+        <v>468</v>
+      </c>
+      <c r="K36" t="s">
+        <v>151</v>
+      </c>
+      <c r="L36" t="s">
+        <v>469</v>
+      </c>
+      <c r="M36" t="s">
+        <v>469</v>
+      </c>
+      <c r="N36" t="s">
+        <v>469</v>
+      </c>
+      <c r="O36" t="s">
+        <v>156</v>
+      </c>
+      <c r="P36" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>156</v>
+      </c>
+      <c r="R36" t="s">
+        <v>470</v>
+      </c>
+      <c r="S36" t="s">
+        <v>470</v>
+      </c>
+      <c r="T36" t="s">
+        <v>471</v>
+      </c>
+      <c r="U36" t="s">
+        <v>153</v>
+      </c>
+      <c r="V36" t="s">
+        <v>472</v>
+      </c>
+      <c r="W36" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -5516,70 +5450,70 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
+        <v>396</v>
+      </c>
+      <c r="C37" t="s">
+        <v>473</v>
+      </c>
+      <c r="D37" t="s">
+        <v>474</v>
+      </c>
+      <c r="E37" t="s">
+        <v>475</v>
+      </c>
+      <c r="F37" t="s">
+        <v>476</v>
+      </c>
+      <c r="G37" t="s">
+        <v>477</v>
+      </c>
+      <c r="H37" t="s">
+        <v>478</v>
+      </c>
+      <c r="I37" t="s">
+        <v>447</v>
+      </c>
+      <c r="J37" t="s">
+        <v>479</v>
+      </c>
+      <c r="K37" t="s">
+        <v>480</v>
+      </c>
+      <c r="L37" t="s">
+        <v>481</v>
+      </c>
+      <c r="M37" t="s">
+        <v>482</v>
+      </c>
+      <c r="N37" t="s">
+        <v>483</v>
+      </c>
+      <c r="O37" t="s">
+        <v>397</v>
+      </c>
+      <c r="P37" t="s">
         <v>484</v>
       </c>
-      <c r="C37" t="s">
+      <c r="Q37" t="s">
         <v>485</v>
       </c>
-      <c r="D37" t="s">
+      <c r="R37" t="s">
         <v>486</v>
       </c>
-      <c r="E37" t="s">
+      <c r="S37" t="s">
         <v>487</v>
       </c>
-      <c r="F37" t="s">
+      <c r="T37" t="s">
         <v>488</v>
       </c>
-      <c r="G37" t="s">
-        <v>488</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="U37" t="s">
         <v>489</v>
       </c>
-      <c r="I37" t="s">
+      <c r="V37" t="s">
         <v>490</v>
       </c>
-      <c r="J37" t="s">
-        <v>490</v>
-      </c>
-      <c r="K37" t="s">
-        <v>151</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="W37" t="s">
         <v>491</v>
-      </c>
-      <c r="M37" t="s">
-        <v>491</v>
-      </c>
-      <c r="N37" t="s">
-        <v>491</v>
-      </c>
-      <c r="O37" t="s">
-        <v>156</v>
-      </c>
-      <c r="P37" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>156</v>
-      </c>
-      <c r="R37" t="s">
-        <v>492</v>
-      </c>
-      <c r="S37" t="s">
-        <v>492</v>
-      </c>
-      <c r="T37" t="s">
-        <v>493</v>
-      </c>
-      <c r="U37" t="s">
-        <v>153</v>
-      </c>
-      <c r="V37" t="s">
-        <v>494</v>
-      </c>
-      <c r="W37" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -5587,70 +5521,70 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>418</v>
+        <v>492</v>
       </c>
       <c r="C38" t="s">
+        <v>493</v>
+      </c>
+      <c r="D38" t="s">
+        <v>494</v>
+      </c>
+      <c r="E38" t="s">
         <v>495</v>
       </c>
-      <c r="D38" t="s">
+      <c r="F38" t="s">
+        <v>456</v>
+      </c>
+      <c r="G38" t="s">
         <v>496</v>
       </c>
-      <c r="E38" t="s">
+      <c r="H38" t="s">
+        <v>496</v>
+      </c>
+      <c r="I38" t="s">
         <v>497</v>
       </c>
-      <c r="F38" t="s">
+      <c r="J38" t="s">
+        <v>497</v>
+      </c>
+      <c r="K38" t="s">
+        <v>497</v>
+      </c>
+      <c r="L38" t="s">
         <v>498</v>
       </c>
-      <c r="G38" t="s">
+      <c r="M38" t="s">
+        <v>498</v>
+      </c>
+      <c r="N38" t="s">
+        <v>498</v>
+      </c>
+      <c r="O38" t="s">
+        <v>456</v>
+      </c>
+      <c r="P38" t="s">
+        <v>496</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>496</v>
+      </c>
+      <c r="R38" t="s">
         <v>499</v>
       </c>
-      <c r="H38" t="s">
+      <c r="S38" t="s">
         <v>500</v>
       </c>
-      <c r="I38" t="s">
-        <v>469</v>
-      </c>
-      <c r="J38" t="s">
+      <c r="T38" t="s">
+        <v>500</v>
+      </c>
+      <c r="U38" t="s">
         <v>501</v>
       </c>
-      <c r="K38" t="s">
+      <c r="V38" t="s">
         <v>502</v>
       </c>
-      <c r="L38" t="s">
-        <v>503</v>
-      </c>
-      <c r="M38" t="s">
-        <v>504</v>
-      </c>
-      <c r="N38" t="s">
-        <v>505</v>
-      </c>
-      <c r="O38" t="s">
-        <v>419</v>
-      </c>
-      <c r="P38" t="s">
-        <v>506</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>507</v>
-      </c>
-      <c r="R38" t="s">
-        <v>508</v>
-      </c>
-      <c r="S38" t="s">
-        <v>509</v>
-      </c>
-      <c r="T38" t="s">
-        <v>510</v>
-      </c>
-      <c r="U38" t="s">
-        <v>511</v>
-      </c>
-      <c r="V38" t="s">
-        <v>512</v>
-      </c>
       <c r="W38" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -5658,70 +5592,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>514</v>
-      </c>
-      <c r="C39" t="s">
-        <v>515</v>
-      </c>
-      <c r="D39" t="s">
-        <v>516</v>
-      </c>
-      <c r="E39" t="s">
-        <v>517</v>
-      </c>
-      <c r="F39" t="s">
-        <v>478</v>
-      </c>
-      <c r="G39" t="s">
-        <v>518</v>
-      </c>
-      <c r="H39" t="s">
-        <v>518</v>
-      </c>
-      <c r="I39" t="s">
-        <v>519</v>
-      </c>
-      <c r="J39" t="s">
-        <v>519</v>
-      </c>
-      <c r="K39" t="s">
-        <v>519</v>
-      </c>
-      <c r="L39" t="s">
-        <v>520</v>
-      </c>
-      <c r="M39" t="s">
-        <v>520</v>
-      </c>
-      <c r="N39" t="s">
-        <v>520</v>
-      </c>
-      <c r="O39" t="s">
-        <v>478</v>
-      </c>
-      <c r="P39" t="s">
-        <v>518</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>518</v>
-      </c>
-      <c r="R39" t="s">
-        <v>521</v>
-      </c>
-      <c r="S39" t="s">
-        <v>522</v>
-      </c>
-      <c r="T39" t="s">
-        <v>522</v>
-      </c>
-      <c r="U39" t="s">
-        <v>523</v>
-      </c>
-      <c r="V39" t="s">
-        <v>524</v>
-      </c>
-      <c r="W39" t="s">
-        <v>524</v>
+        <v>503</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
@@ -5729,7 +5600,70 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>525</v>
+        <v>462</v>
+      </c>
+      <c r="C40" t="s">
+        <v>504</v>
+      </c>
+      <c r="D40" t="s">
+        <v>505</v>
+      </c>
+      <c r="E40" t="s">
+        <v>506</v>
+      </c>
+      <c r="F40" t="s">
+        <v>152</v>
+      </c>
+      <c r="G40" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" t="s">
+        <v>355</v>
+      </c>
+      <c r="I40" t="s">
+        <v>507</v>
+      </c>
+      <c r="J40" t="s">
+        <v>346</v>
+      </c>
+      <c r="K40" t="s">
+        <v>346</v>
+      </c>
+      <c r="L40" t="s">
+        <v>348</v>
+      </c>
+      <c r="M40" t="s">
+        <v>348</v>
+      </c>
+      <c r="N40" t="s">
+        <v>348</v>
+      </c>
+      <c r="O40" t="s">
+        <v>353</v>
+      </c>
+      <c r="P40" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>353</v>
+      </c>
+      <c r="R40" t="s">
+        <v>508</v>
+      </c>
+      <c r="S40" t="s">
+        <v>509</v>
+      </c>
+      <c r="T40" t="s">
+        <v>510</v>
+      </c>
+      <c r="U40" t="s">
+        <v>511</v>
+      </c>
+      <c r="V40" t="s">
+        <v>511</v>
+      </c>
+      <c r="W40" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
@@ -5737,70 +5671,70 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>484</v>
+        <v>396</v>
       </c>
       <c r="C41" t="s">
+        <v>512</v>
+      </c>
+      <c r="D41" t="s">
+        <v>297</v>
+      </c>
+      <c r="E41" t="s">
+        <v>513</v>
+      </c>
+      <c r="F41" t="s">
+        <v>514</v>
+      </c>
+      <c r="G41" t="s">
+        <v>515</v>
+      </c>
+      <c r="H41" t="s">
+        <v>516</v>
+      </c>
+      <c r="I41" t="s">
+        <v>517</v>
+      </c>
+      <c r="J41" t="s">
+        <v>518</v>
+      </c>
+      <c r="K41" t="s">
+        <v>519</v>
+      </c>
+      <c r="L41" t="s">
+        <v>520</v>
+      </c>
+      <c r="M41" t="s">
+        <v>521</v>
+      </c>
+      <c r="N41" t="s">
+        <v>522</v>
+      </c>
+      <c r="O41" t="s">
+        <v>523</v>
+      </c>
+      <c r="P41" t="s">
+        <v>524</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>525</v>
+      </c>
+      <c r="R41" t="s">
         <v>526</v>
       </c>
-      <c r="D41" t="s">
+      <c r="S41" t="s">
         <v>527</v>
       </c>
-      <c r="E41" t="s">
+      <c r="T41" t="s">
         <v>528</v>
       </c>
-      <c r="F41" t="s">
-        <v>152</v>
-      </c>
-      <c r="G41" t="s">
-        <v>152</v>
-      </c>
-      <c r="H41" t="s">
-        <v>355</v>
-      </c>
-      <c r="I41" t="s">
+      <c r="U41" t="s">
         <v>529</v>
       </c>
-      <c r="J41" t="s">
-        <v>346</v>
-      </c>
-      <c r="K41" t="s">
-        <v>346</v>
-      </c>
-      <c r="L41" t="s">
-        <v>348</v>
-      </c>
-      <c r="M41" t="s">
-        <v>348</v>
-      </c>
-      <c r="N41" t="s">
-        <v>348</v>
-      </c>
-      <c r="O41" t="s">
-        <v>353</v>
-      </c>
-      <c r="P41" t="s">
-        <v>353</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>353</v>
-      </c>
-      <c r="R41" t="s">
+      <c r="V41" t="s">
         <v>530</v>
       </c>
-      <c r="S41" t="s">
+      <c r="W41" t="s">
         <v>531</v>
-      </c>
-      <c r="T41" t="s">
-        <v>532</v>
-      </c>
-      <c r="U41" t="s">
-        <v>533</v>
-      </c>
-      <c r="V41" t="s">
-        <v>533</v>
-      </c>
-      <c r="W41" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
@@ -5808,13 +5742,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>418</v>
+        <v>532</v>
       </c>
       <c r="C42" t="s">
+        <v>533</v>
+      </c>
+      <c r="D42" t="s">
         <v>534</v>
-      </c>
-      <c r="D42" t="s">
-        <v>297</v>
       </c>
       <c r="E42" t="s">
         <v>535</v>
@@ -5894,55 +5828,55 @@
         <v>558</v>
       </c>
       <c r="G43" t="s">
+        <v>242</v>
+      </c>
+      <c r="H43" t="s">
         <v>559</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>560</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>561</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>562</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>563</v>
       </c>
-      <c r="L43" t="s">
+      <c r="M43" t="s">
         <v>564</v>
       </c>
-      <c r="M43" t="s">
+      <c r="N43" t="s">
         <v>565</v>
       </c>
-      <c r="N43" t="s">
+      <c r="O43" t="s">
         <v>566</v>
       </c>
-      <c r="O43" t="s">
+      <c r="P43" t="s">
         <v>567</v>
       </c>
-      <c r="P43" t="s">
+      <c r="Q43" t="s">
         <v>568</v>
       </c>
-      <c r="Q43" t="s">
+      <c r="R43" t="s">
         <v>569</v>
       </c>
-      <c r="R43" t="s">
+      <c r="S43" t="s">
         <v>570</v>
       </c>
-      <c r="S43" t="s">
+      <c r="T43" t="s">
         <v>571</v>
       </c>
-      <c r="T43" t="s">
+      <c r="U43" t="s">
         <v>572</v>
       </c>
-      <c r="U43" t="s">
+      <c r="V43" t="s">
         <v>573</v>
       </c>
-      <c r="V43" t="s">
+      <c r="W43" t="s">
         <v>574</v>
-      </c>
-      <c r="W43" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
@@ -5950,70 +5884,70 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
+        <v>575</v>
+      </c>
+      <c r="C44" t="s">
+        <v>575</v>
+      </c>
+      <c r="D44" t="s">
+        <v>575</v>
+      </c>
+      <c r="E44" t="s">
+        <v>575</v>
+      </c>
+      <c r="F44" t="s">
+        <v>575</v>
+      </c>
+      <c r="G44" t="s">
+        <v>575</v>
+      </c>
+      <c r="H44" t="s">
+        <v>575</v>
+      </c>
+      <c r="I44" t="s">
+        <v>575</v>
+      </c>
+      <c r="J44" t="s">
+        <v>575</v>
+      </c>
+      <c r="K44" t="s">
+        <v>575</v>
+      </c>
+      <c r="L44" t="s">
+        <v>575</v>
+      </c>
+      <c r="M44" t="s">
+        <v>575</v>
+      </c>
+      <c r="N44" t="s">
+        <v>575</v>
+      </c>
+      <c r="O44" t="s">
         <v>576</v>
       </c>
-      <c r="C44" t="s">
-        <v>577</v>
-      </c>
-      <c r="D44" t="s">
-        <v>578</v>
-      </c>
-      <c r="E44" t="s">
-        <v>579</v>
-      </c>
-      <c r="F44" t="s">
-        <v>580</v>
-      </c>
-      <c r="G44" t="s">
-        <v>242</v>
-      </c>
-      <c r="H44" t="s">
-        <v>581</v>
-      </c>
-      <c r="I44" t="s">
-        <v>582</v>
-      </c>
-      <c r="J44" t="s">
-        <v>583</v>
-      </c>
-      <c r="K44" t="s">
-        <v>584</v>
-      </c>
-      <c r="L44" t="s">
-        <v>585</v>
-      </c>
-      <c r="M44" t="s">
-        <v>586</v>
-      </c>
-      <c r="N44" t="s">
-        <v>587</v>
-      </c>
-      <c r="O44" t="s">
-        <v>588</v>
-      </c>
       <c r="P44" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="Q44" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
       <c r="R44" t="s">
-        <v>591</v>
+        <v>576</v>
       </c>
       <c r="S44" t="s">
-        <v>592</v>
+        <v>576</v>
       </c>
       <c r="T44" t="s">
-        <v>593</v>
+        <v>576</v>
       </c>
       <c r="U44" t="s">
-        <v>594</v>
+        <v>576</v>
       </c>
       <c r="V44" t="s">
-        <v>595</v>
+        <v>576</v>
       </c>
       <c r="W44" t="s">
-        <v>596</v>
+        <v>576</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
@@ -6021,67 +5955,67 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
+        <v>577</v>
+      </c>
+      <c r="C45" t="s">
+        <v>578</v>
+      </c>
+      <c r="D45" t="s">
+        <v>579</v>
+      </c>
+      <c r="E45" t="s">
+        <v>580</v>
+      </c>
+      <c r="F45" t="s">
+        <v>581</v>
+      </c>
+      <c r="G45" t="s">
+        <v>582</v>
+      </c>
+      <c r="H45" t="s">
+        <v>583</v>
+      </c>
+      <c r="I45" t="s">
+        <v>584</v>
+      </c>
+      <c r="J45" t="s">
+        <v>585</v>
+      </c>
+      <c r="K45" t="s">
+        <v>586</v>
+      </c>
+      <c r="L45" t="s">
+        <v>587</v>
+      </c>
+      <c r="M45" t="s">
+        <v>588</v>
+      </c>
+      <c r="N45" t="s">
+        <v>589</v>
+      </c>
+      <c r="O45" t="s">
+        <v>590</v>
+      </c>
+      <c r="P45" t="s">
+        <v>591</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>592</v>
+      </c>
+      <c r="R45" t="s">
+        <v>593</v>
+      </c>
+      <c r="S45" t="s">
+        <v>594</v>
+      </c>
+      <c r="T45" t="s">
+        <v>595</v>
+      </c>
+      <c r="U45" t="s">
+        <v>596</v>
+      </c>
+      <c r="V45" t="s">
         <v>597</v>
-      </c>
-      <c r="C45" t="s">
-        <v>597</v>
-      </c>
-      <c r="D45" t="s">
-        <v>597</v>
-      </c>
-      <c r="E45" t="s">
-        <v>597</v>
-      </c>
-      <c r="F45" t="s">
-        <v>597</v>
-      </c>
-      <c r="G45" t="s">
-        <v>597</v>
-      </c>
-      <c r="H45" t="s">
-        <v>597</v>
-      </c>
-      <c r="I45" t="s">
-        <v>597</v>
-      </c>
-      <c r="J45" t="s">
-        <v>597</v>
-      </c>
-      <c r="K45" t="s">
-        <v>597</v>
-      </c>
-      <c r="L45" t="s">
-        <v>597</v>
-      </c>
-      <c r="M45" t="s">
-        <v>597</v>
-      </c>
-      <c r="N45" t="s">
-        <v>597</v>
-      </c>
-      <c r="O45" t="s">
-        <v>598</v>
-      </c>
-      <c r="P45" t="s">
-        <v>598</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>598</v>
-      </c>
-      <c r="R45" t="s">
-        <v>598</v>
-      </c>
-      <c r="S45" t="s">
-        <v>598</v>
-      </c>
-      <c r="T45" t="s">
-        <v>598</v>
-      </c>
-      <c r="U45" t="s">
-        <v>598</v>
-      </c>
-      <c r="V45" t="s">
-        <v>598</v>
       </c>
       <c r="W45" t="s">
         <v>598</v>
@@ -6181,52 +6115,52 @@
         <v>626</v>
       </c>
       <c r="H47" t="s">
+        <v>625</v>
+      </c>
+      <c r="I47" t="s">
+        <v>47</v>
+      </c>
+      <c r="J47" t="s">
+        <v>43</v>
+      </c>
+      <c r="K47" t="s">
         <v>627</v>
       </c>
-      <c r="I47" t="s">
+      <c r="L47" t="s">
+        <v>48</v>
+      </c>
+      <c r="M47" t="s">
         <v>628</v>
       </c>
-      <c r="J47" t="s">
+      <c r="N47" t="s">
         <v>629</v>
       </c>
-      <c r="K47" t="s">
+      <c r="O47" t="s">
         <v>630</v>
       </c>
-      <c r="L47" t="s">
+      <c r="P47" t="s">
         <v>631</v>
       </c>
-      <c r="M47" t="s">
+      <c r="Q47" t="s">
         <v>632</v>
       </c>
-      <c r="N47" t="s">
+      <c r="R47" t="s">
         <v>633</v>
       </c>
-      <c r="O47" t="s">
+      <c r="S47" t="s">
         <v>634</v>
       </c>
-      <c r="P47" t="s">
+      <c r="T47" t="s">
         <v>635</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="U47" t="s">
         <v>636</v>
       </c>
-      <c r="R47" t="s">
+      <c r="V47" t="s">
+        <v>405</v>
+      </c>
+      <c r="W47" t="s">
         <v>637</v>
-      </c>
-      <c r="S47" t="s">
-        <v>638</v>
-      </c>
-      <c r="T47" t="s">
-        <v>639</v>
-      </c>
-      <c r="U47" t="s">
-        <v>640</v>
-      </c>
-      <c r="V47" t="s">
-        <v>641</v>
-      </c>
-      <c r="W47" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
@@ -6234,70 +6168,70 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
+        <v>638</v>
+      </c>
+      <c r="C48" t="s">
+        <v>639</v>
+      </c>
+      <c r="D48" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" t="s">
+        <v>640</v>
+      </c>
+      <c r="F48" t="s">
+        <v>641</v>
+      </c>
+      <c r="G48" t="s">
+        <v>373</v>
+      </c>
+      <c r="H48" t="s">
+        <v>68</v>
+      </c>
+      <c r="I48" t="s">
+        <v>365</v>
+      </c>
+      <c r="J48" t="s">
+        <v>642</v>
+      </c>
+      <c r="K48" t="s">
+        <v>374</v>
+      </c>
+      <c r="L48" t="s">
         <v>643</v>
       </c>
-      <c r="C48" t="s">
+      <c r="M48" t="s">
         <v>644</v>
       </c>
-      <c r="D48" t="s">
+      <c r="N48" t="s">
+        <v>60</v>
+      </c>
+      <c r="O48" t="s">
         <v>645</v>
       </c>
-      <c r="E48" t="s">
+      <c r="P48" t="s">
+        <v>350</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>59</v>
+      </c>
+      <c r="R48" t="s">
+        <v>204</v>
+      </c>
+      <c r="S48" t="s">
         <v>646</v>
       </c>
-      <c r="F48" t="s">
+      <c r="T48" t="s">
+        <v>140</v>
+      </c>
+      <c r="U48" t="s">
+        <v>368</v>
+      </c>
+      <c r="V48" t="s">
         <v>647</v>
       </c>
-      <c r="G48" t="s">
+      <c r="W48" t="s">
         <v>648</v>
-      </c>
-      <c r="H48" t="s">
-        <v>647</v>
-      </c>
-      <c r="I48" t="s">
-        <v>47</v>
-      </c>
-      <c r="J48" t="s">
-        <v>43</v>
-      </c>
-      <c r="K48" t="s">
-        <v>649</v>
-      </c>
-      <c r="L48" t="s">
-        <v>48</v>
-      </c>
-      <c r="M48" t="s">
-        <v>650</v>
-      </c>
-      <c r="N48" t="s">
-        <v>651</v>
-      </c>
-      <c r="O48" t="s">
-        <v>652</v>
-      </c>
-      <c r="P48" t="s">
-        <v>653</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>654</v>
-      </c>
-      <c r="R48" t="s">
-        <v>655</v>
-      </c>
-      <c r="S48" t="s">
-        <v>656</v>
-      </c>
-      <c r="T48" t="s">
-        <v>657</v>
-      </c>
-      <c r="U48" t="s">
-        <v>658</v>
-      </c>
-      <c r="V48" t="s">
-        <v>427</v>
-      </c>
-      <c r="W48" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
@@ -6305,70 +6239,70 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>660</v>
+        <v>649</v>
       </c>
       <c r="C49" t="s">
-        <v>661</v>
+        <v>649</v>
       </c>
       <c r="D49" t="s">
-        <v>72</v>
+        <v>649</v>
       </c>
       <c r="E49" t="s">
-        <v>662</v>
+        <v>649</v>
       </c>
       <c r="F49" t="s">
-        <v>663</v>
+        <v>649</v>
       </c>
       <c r="G49" t="s">
-        <v>373</v>
+        <v>649</v>
       </c>
       <c r="H49" t="s">
-        <v>68</v>
+        <v>649</v>
       </c>
       <c r="I49" t="s">
-        <v>365</v>
+        <v>649</v>
       </c>
       <c r="J49" t="s">
-        <v>664</v>
+        <v>649</v>
       </c>
       <c r="K49" t="s">
-        <v>374</v>
+        <v>649</v>
       </c>
       <c r="L49" t="s">
-        <v>665</v>
+        <v>649</v>
       </c>
       <c r="M49" t="s">
-        <v>666</v>
+        <v>649</v>
       </c>
       <c r="N49" t="s">
-        <v>60</v>
+        <v>649</v>
       </c>
       <c r="O49" t="s">
-        <v>667</v>
+        <v>650</v>
       </c>
       <c r="P49" t="s">
-        <v>350</v>
+        <v>650</v>
       </c>
       <c r="Q49" t="s">
-        <v>59</v>
+        <v>650</v>
       </c>
       <c r="R49" t="s">
-        <v>204</v>
+        <v>650</v>
       </c>
       <c r="S49" t="s">
-        <v>668</v>
+        <v>650</v>
       </c>
       <c r="T49" t="s">
-        <v>140</v>
+        <v>650</v>
       </c>
       <c r="U49" t="s">
-        <v>368</v>
+        <v>650</v>
       </c>
       <c r="V49" t="s">
-        <v>669</v>
+        <v>650</v>
       </c>
       <c r="W49" t="s">
-        <v>670</v>
+        <v>650</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
@@ -6376,67 +6310,67 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
+        <v>651</v>
+      </c>
+      <c r="C50" t="s">
+        <v>652</v>
+      </c>
+      <c r="D50" t="s">
+        <v>653</v>
+      </c>
+      <c r="E50" t="s">
+        <v>654</v>
+      </c>
+      <c r="F50" t="s">
+        <v>655</v>
+      </c>
+      <c r="G50" t="s">
+        <v>656</v>
+      </c>
+      <c r="H50" t="s">
+        <v>657</v>
+      </c>
+      <c r="I50" t="s">
+        <v>658</v>
+      </c>
+      <c r="J50" t="s">
+        <v>659</v>
+      </c>
+      <c r="K50" t="s">
+        <v>660</v>
+      </c>
+      <c r="L50" t="s">
+        <v>661</v>
+      </c>
+      <c r="M50" t="s">
+        <v>662</v>
+      </c>
+      <c r="N50" t="s">
+        <v>663</v>
+      </c>
+      <c r="O50" t="s">
+        <v>664</v>
+      </c>
+      <c r="P50" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>666</v>
+      </c>
+      <c r="R50" t="s">
+        <v>667</v>
+      </c>
+      <c r="S50" t="s">
+        <v>668</v>
+      </c>
+      <c r="T50" t="s">
+        <v>669</v>
+      </c>
+      <c r="U50" t="s">
+        <v>670</v>
+      </c>
+      <c r="V50" t="s">
         <v>671</v>
-      </c>
-      <c r="C50" t="s">
-        <v>671</v>
-      </c>
-      <c r="D50" t="s">
-        <v>671</v>
-      </c>
-      <c r="E50" t="s">
-        <v>671</v>
-      </c>
-      <c r="F50" t="s">
-        <v>671</v>
-      </c>
-      <c r="G50" t="s">
-        <v>671</v>
-      </c>
-      <c r="H50" t="s">
-        <v>671</v>
-      </c>
-      <c r="I50" t="s">
-        <v>671</v>
-      </c>
-      <c r="J50" t="s">
-        <v>671</v>
-      </c>
-      <c r="K50" t="s">
-        <v>671</v>
-      </c>
-      <c r="L50" t="s">
-        <v>671</v>
-      </c>
-      <c r="M50" t="s">
-        <v>671</v>
-      </c>
-      <c r="N50" t="s">
-        <v>671</v>
-      </c>
-      <c r="O50" t="s">
-        <v>672</v>
-      </c>
-      <c r="P50" t="s">
-        <v>672</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>672</v>
-      </c>
-      <c r="R50" t="s">
-        <v>672</v>
-      </c>
-      <c r="S50" t="s">
-        <v>672</v>
-      </c>
-      <c r="T50" t="s">
-        <v>672</v>
-      </c>
-      <c r="U50" t="s">
-        <v>672</v>
-      </c>
-      <c r="V50" t="s">
-        <v>672</v>
       </c>
       <c r="W50" t="s">
         <v>672</v>
@@ -6450,67 +6384,67 @@
         <v>673</v>
       </c>
       <c r="C51" t="s">
+        <v>673</v>
+      </c>
+      <c r="D51" t="s">
+        <v>673</v>
+      </c>
+      <c r="E51" t="s">
+        <v>673</v>
+      </c>
+      <c r="F51" t="s">
+        <v>673</v>
+      </c>
+      <c r="G51" t="s">
+        <v>673</v>
+      </c>
+      <c r="H51" t="s">
+        <v>673</v>
+      </c>
+      <c r="I51" t="s">
+        <v>673</v>
+      </c>
+      <c r="J51" t="s">
+        <v>673</v>
+      </c>
+      <c r="K51" t="s">
+        <v>673</v>
+      </c>
+      <c r="L51" t="s">
+        <v>673</v>
+      </c>
+      <c r="M51" t="s">
+        <v>673</v>
+      </c>
+      <c r="N51" t="s">
+        <v>673</v>
+      </c>
+      <c r="O51" t="s">
         <v>674</v>
       </c>
-      <c r="D51" t="s">
-        <v>675</v>
-      </c>
-      <c r="E51" t="s">
-        <v>676</v>
-      </c>
-      <c r="F51" t="s">
-        <v>677</v>
-      </c>
-      <c r="G51" t="s">
-        <v>678</v>
-      </c>
-      <c r="H51" t="s">
-        <v>679</v>
-      </c>
-      <c r="I51" t="s">
-        <v>680</v>
-      </c>
-      <c r="J51" t="s">
-        <v>681</v>
-      </c>
-      <c r="K51" t="s">
-        <v>682</v>
-      </c>
-      <c r="L51" t="s">
-        <v>683</v>
-      </c>
-      <c r="M51" t="s">
-        <v>684</v>
-      </c>
-      <c r="N51" t="s">
-        <v>685</v>
-      </c>
-      <c r="O51" t="s">
-        <v>686</v>
-      </c>
       <c r="P51" t="s">
-        <v>687</v>
+        <v>674</v>
       </c>
       <c r="Q51" t="s">
-        <v>688</v>
+        <v>674</v>
       </c>
       <c r="R51" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="S51" t="s">
-        <v>690</v>
+        <v>674</v>
       </c>
       <c r="T51" t="s">
-        <v>691</v>
+        <v>674</v>
       </c>
       <c r="U51" t="s">
-        <v>692</v>
+        <v>674</v>
       </c>
       <c r="V51" t="s">
-        <v>693</v>
+        <v>674</v>
       </c>
       <c r="W51" t="s">
-        <v>694</v>
+        <v>674</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
@@ -6518,70 +6452,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>695</v>
-      </c>
-      <c r="C52" t="s">
-        <v>695</v>
-      </c>
-      <c r="D52" t="s">
-        <v>695</v>
-      </c>
-      <c r="E52" t="s">
-        <v>695</v>
-      </c>
-      <c r="F52" t="s">
-        <v>695</v>
-      </c>
-      <c r="G52" t="s">
-        <v>695</v>
-      </c>
-      <c r="H52" t="s">
-        <v>695</v>
-      </c>
-      <c r="I52" t="s">
-        <v>695</v>
-      </c>
-      <c r="J52" t="s">
-        <v>695</v>
-      </c>
-      <c r="K52" t="s">
-        <v>695</v>
-      </c>
-      <c r="L52" t="s">
-        <v>695</v>
-      </c>
-      <c r="M52" t="s">
-        <v>695</v>
-      </c>
-      <c r="N52" t="s">
-        <v>695</v>
-      </c>
-      <c r="O52" t="s">
-        <v>696</v>
-      </c>
-      <c r="P52" t="s">
-        <v>696</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>696</v>
-      </c>
-      <c r="R52" t="s">
-        <v>696</v>
-      </c>
-      <c r="S52" t="s">
-        <v>696</v>
-      </c>
-      <c r="T52" t="s">
-        <v>696</v>
-      </c>
-      <c r="U52" t="s">
-        <v>696</v>
-      </c>
-      <c r="V52" t="s">
-        <v>696</v>
-      </c>
-      <c r="W52" t="s">
-        <v>696</v>
+        <v>675</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
@@ -6589,7 +6460,70 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>697</v>
+        <v>676</v>
+      </c>
+      <c r="C53" t="s">
+        <v>677</v>
+      </c>
+      <c r="D53" t="s">
+        <v>677</v>
+      </c>
+      <c r="E53" t="s">
+        <v>677</v>
+      </c>
+      <c r="F53" t="s">
+        <v>677</v>
+      </c>
+      <c r="G53" t="s">
+        <v>677</v>
+      </c>
+      <c r="H53" t="s">
+        <v>677</v>
+      </c>
+      <c r="I53" t="s">
+        <v>677</v>
+      </c>
+      <c r="J53" t="s">
+        <v>677</v>
+      </c>
+      <c r="K53" t="s">
+        <v>677</v>
+      </c>
+      <c r="L53" t="s">
+        <v>677</v>
+      </c>
+      <c r="M53" t="s">
+        <v>677</v>
+      </c>
+      <c r="N53" t="s">
+        <v>677</v>
+      </c>
+      <c r="O53" t="s">
+        <v>455</v>
+      </c>
+      <c r="P53" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>455</v>
+      </c>
+      <c r="R53" t="s">
+        <v>677</v>
+      </c>
+      <c r="S53" t="s">
+        <v>455</v>
+      </c>
+      <c r="T53" t="s">
+        <v>455</v>
+      </c>
+      <c r="U53" t="s">
+        <v>677</v>
+      </c>
+      <c r="V53" t="s">
+        <v>677</v>
+      </c>
+      <c r="W53" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
@@ -6597,70 +6531,70 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>698</v>
+        <v>678</v>
       </c>
       <c r="C54" t="s">
-        <v>699</v>
+        <v>679</v>
       </c>
       <c r="D54" t="s">
-        <v>699</v>
+        <v>680</v>
       </c>
       <c r="E54" t="s">
-        <v>699</v>
+        <v>681</v>
       </c>
       <c r="F54" t="s">
-        <v>699</v>
+        <v>682</v>
       </c>
       <c r="G54" t="s">
-        <v>699</v>
+        <v>683</v>
       </c>
       <c r="H54" t="s">
-        <v>699</v>
+        <v>684</v>
       </c>
       <c r="I54" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
       <c r="J54" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="K54" t="s">
-        <v>699</v>
+        <v>687</v>
       </c>
       <c r="L54" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
       <c r="M54" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="N54" t="s">
-        <v>699</v>
+        <v>690</v>
       </c>
       <c r="O54" t="s">
-        <v>477</v>
+        <v>691</v>
       </c>
       <c r="P54" t="s">
-        <v>477</v>
+        <v>692</v>
       </c>
       <c r="Q54" t="s">
-        <v>477</v>
+        <v>502</v>
       </c>
       <c r="R54" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="S54" t="s">
-        <v>477</v>
+        <v>494</v>
       </c>
       <c r="T54" t="s">
-        <v>477</v>
+        <v>694</v>
       </c>
       <c r="U54" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="V54" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
       <c r="W54" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
@@ -6668,70 +6602,70 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
+        <v>697</v>
+      </c>
+      <c r="C55" t="s">
+        <v>698</v>
+      </c>
+      <c r="D55" t="s">
+        <v>699</v>
+      </c>
+      <c r="E55" t="s">
         <v>700</v>
       </c>
-      <c r="C55" t="s">
+      <c r="F55" t="s">
+        <v>457</v>
+      </c>
+      <c r="G55" t="s">
+        <v>457</v>
+      </c>
+      <c r="H55" t="s">
+        <v>692</v>
+      </c>
+      <c r="I55" t="s">
+        <v>335</v>
+      </c>
+      <c r="J55" t="s">
+        <v>500</v>
+      </c>
+      <c r="K55" t="s">
+        <v>339</v>
+      </c>
+      <c r="L55" t="s">
         <v>701</v>
       </c>
-      <c r="D55" t="s">
+      <c r="M55" t="s">
         <v>702</v>
       </c>
-      <c r="E55" t="s">
+      <c r="N55" t="s">
         <v>703</v>
       </c>
-      <c r="F55" t="s">
+      <c r="O55" t="s">
         <v>704</v>
       </c>
-      <c r="G55" t="s">
+      <c r="P55" t="s">
         <v>705</v>
       </c>
-      <c r="H55" t="s">
+      <c r="Q55" t="s">
+        <v>704</v>
+      </c>
+      <c r="R55" t="s">
         <v>706</v>
       </c>
-      <c r="I55" t="s">
+      <c r="S55" t="s">
         <v>707</v>
       </c>
-      <c r="J55" t="s">
+      <c r="T55" t="s">
         <v>708</v>
       </c>
-      <c r="K55" t="s">
+      <c r="U55" t="s">
+        <v>502</v>
+      </c>
+      <c r="V55" t="s">
         <v>709</v>
       </c>
-      <c r="L55" t="s">
-        <v>710</v>
-      </c>
-      <c r="M55" t="s">
-        <v>711</v>
-      </c>
-      <c r="N55" t="s">
-        <v>712</v>
-      </c>
-      <c r="O55" t="s">
-        <v>713</v>
-      </c>
-      <c r="P55" t="s">
-        <v>714</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>524</v>
-      </c>
-      <c r="R55" t="s">
-        <v>715</v>
-      </c>
-      <c r="S55" t="s">
-        <v>516</v>
-      </c>
-      <c r="T55" t="s">
-        <v>716</v>
-      </c>
-      <c r="U55" t="s">
-        <v>717</v>
-      </c>
-      <c r="V55" t="s">
-        <v>710</v>
-      </c>
       <c r="W55" t="s">
-        <v>718</v>
+        <v>501</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
@@ -6739,70 +6673,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>719</v>
-      </c>
-      <c r="C56" t="s">
-        <v>720</v>
-      </c>
-      <c r="D56" t="s">
-        <v>721</v>
-      </c>
-      <c r="E56" t="s">
-        <v>722</v>
-      </c>
-      <c r="F56" t="s">
-        <v>479</v>
-      </c>
-      <c r="G56" t="s">
-        <v>479</v>
-      </c>
-      <c r="H56" t="s">
-        <v>714</v>
-      </c>
-      <c r="I56" t="s">
-        <v>335</v>
-      </c>
-      <c r="J56" t="s">
-        <v>522</v>
-      </c>
-      <c r="K56" t="s">
-        <v>339</v>
-      </c>
-      <c r="L56" t="s">
-        <v>723</v>
-      </c>
-      <c r="M56" t="s">
-        <v>724</v>
-      </c>
-      <c r="N56" t="s">
-        <v>725</v>
-      </c>
-      <c r="O56" t="s">
-        <v>726</v>
-      </c>
-      <c r="P56" t="s">
-        <v>727</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>726</v>
-      </c>
-      <c r="R56" t="s">
-        <v>728</v>
-      </c>
-      <c r="S56" t="s">
-        <v>729</v>
-      </c>
-      <c r="T56" t="s">
-        <v>730</v>
-      </c>
-      <c r="U56" t="s">
-        <v>524</v>
-      </c>
-      <c r="V56" t="s">
-        <v>731</v>
-      </c>
-      <c r="W56" t="s">
-        <v>523</v>
+        <v>710</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
@@ -6810,7 +6681,70 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>732</v>
+        <v>676</v>
+      </c>
+      <c r="C57" t="s">
+        <v>677</v>
+      </c>
+      <c r="D57" t="s">
+        <v>677</v>
+      </c>
+      <c r="E57" t="s">
+        <v>677</v>
+      </c>
+      <c r="F57" t="s">
+        <v>677</v>
+      </c>
+      <c r="G57" t="s">
+        <v>677</v>
+      </c>
+      <c r="H57" t="s">
+        <v>677</v>
+      </c>
+      <c r="I57" t="s">
+        <v>677</v>
+      </c>
+      <c r="J57" t="s">
+        <v>677</v>
+      </c>
+      <c r="K57" t="s">
+        <v>677</v>
+      </c>
+      <c r="L57" t="s">
+        <v>677</v>
+      </c>
+      <c r="M57" t="s">
+        <v>677</v>
+      </c>
+      <c r="N57" t="s">
+        <v>677</v>
+      </c>
+      <c r="O57" t="s">
+        <v>711</v>
+      </c>
+      <c r="P57" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>711</v>
+      </c>
+      <c r="R57" t="s">
+        <v>677</v>
+      </c>
+      <c r="S57" t="s">
+        <v>711</v>
+      </c>
+      <c r="T57" t="s">
+        <v>711</v>
+      </c>
+      <c r="U57" t="s">
+        <v>677</v>
+      </c>
+      <c r="V57" t="s">
+        <v>677</v>
+      </c>
+      <c r="W57" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
@@ -6818,70 +6752,70 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>698</v>
+        <v>678</v>
       </c>
       <c r="C58" t="s">
-        <v>699</v>
+        <v>712</v>
       </c>
       <c r="D58" t="s">
-        <v>699</v>
+        <v>713</v>
       </c>
       <c r="E58" t="s">
-        <v>699</v>
+        <v>714</v>
       </c>
       <c r="F58" t="s">
-        <v>699</v>
+        <v>715</v>
       </c>
       <c r="G58" t="s">
-        <v>699</v>
+        <v>716</v>
       </c>
       <c r="H58" t="s">
-        <v>699</v>
+        <v>592</v>
       </c>
       <c r="I58" t="s">
-        <v>699</v>
+        <v>717</v>
       </c>
       <c r="J58" t="s">
-        <v>699</v>
+        <v>718</v>
       </c>
       <c r="K58" t="s">
-        <v>699</v>
+        <v>719</v>
       </c>
       <c r="L58" t="s">
-        <v>699</v>
+        <v>720</v>
       </c>
       <c r="M58" t="s">
-        <v>699</v>
+        <v>721</v>
       </c>
       <c r="N58" t="s">
-        <v>699</v>
+        <v>722</v>
       </c>
       <c r="O58" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
       <c r="P58" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
       <c r="Q58" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="R58" t="s">
-        <v>699</v>
+        <v>726</v>
       </c>
       <c r="S58" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="T58" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="U58" t="s">
-        <v>699</v>
+        <v>729</v>
       </c>
       <c r="V58" t="s">
-        <v>699</v>
+        <v>730</v>
       </c>
       <c r="W58" t="s">
-        <v>699</v>
+        <v>731</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
@@ -6889,25 +6823,25 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>700</v>
+        <v>732</v>
       </c>
       <c r="C59" t="s">
+        <v>733</v>
+      </c>
+      <c r="D59" t="s">
         <v>734</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>735</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>736</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>737</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>738</v>
-      </c>
-      <c r="H59" t="s">
-        <v>614</v>
       </c>
       <c r="I59" t="s">
         <v>739</v>
@@ -6963,67 +6897,40 @@
         <v>754</v>
       </c>
       <c r="C60" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D60" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="E60" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="F60" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="G60" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="H60" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="I60" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="J60" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="K60" t="s">
-        <v>763</v>
+        <v>754</v>
       </c>
       <c r="L60" t="s">
-        <v>764</v>
+        <v>754</v>
       </c>
       <c r="M60" t="s">
-        <v>765</v>
+        <v>754</v>
       </c>
       <c r="N60" t="s">
-        <v>766</v>
-      </c>
-      <c r="O60" t="s">
-        <v>767</v>
-      </c>
-      <c r="P60" t="s">
-        <v>768</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>769</v>
-      </c>
-      <c r="R60" t="s">
-        <v>770</v>
-      </c>
-      <c r="S60" t="s">
-        <v>771</v>
-      </c>
-      <c r="T60" t="s">
-        <v>772</v>
-      </c>
-      <c r="U60" t="s">
-        <v>773</v>
-      </c>
-      <c r="V60" t="s">
-        <v>774</v>
-      </c>
-      <c r="W60" t="s">
-        <v>775</v>
+        <v>754</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.25">
@@ -7031,42 +6938,69 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>776</v>
+        <v>755</v>
       </c>
       <c r="C61" t="s">
-        <v>776</v>
+        <v>756</v>
       </c>
       <c r="D61" t="s">
-        <v>776</v>
+        <v>757</v>
       </c>
       <c r="E61" t="s">
-        <v>776</v>
+        <v>758</v>
       </c>
       <c r="F61" t="s">
-        <v>776</v>
+        <v>759</v>
       </c>
       <c r="G61" t="s">
-        <v>776</v>
+        <v>760</v>
       </c>
       <c r="H61" t="s">
-        <v>776</v>
+        <v>761</v>
       </c>
       <c r="I61" t="s">
-        <v>776</v>
+        <v>762</v>
       </c>
       <c r="J61" t="s">
-        <v>776</v>
+        <v>763</v>
       </c>
       <c r="K61" t="s">
-        <v>776</v>
+        <v>764</v>
       </c>
       <c r="L61" t="s">
-        <v>776</v>
+        <v>765</v>
       </c>
       <c r="M61" t="s">
-        <v>776</v>
+        <v>766</v>
       </c>
       <c r="N61" t="s">
+        <v>767</v>
+      </c>
+      <c r="O61" t="s">
+        <v>768</v>
+      </c>
+      <c r="P61" t="s">
+        <v>769</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>770</v>
+      </c>
+      <c r="R61" t="s">
+        <v>771</v>
+      </c>
+      <c r="S61" t="s">
+        <v>772</v>
+      </c>
+      <c r="T61" t="s">
+        <v>773</v>
+      </c>
+      <c r="U61" t="s">
+        <v>774</v>
+      </c>
+      <c r="V61" t="s">
+        <v>775</v>
+      </c>
+      <c r="W61" t="s">
         <v>776</v>
       </c>
     </row>
@@ -7077,76 +7011,76 @@
       <c r="B62" t="s">
         <v>777</v>
       </c>
-      <c r="C62" t="s">
-        <v>778</v>
-      </c>
-      <c r="D62" t="s">
-        <v>779</v>
-      </c>
-      <c r="E62" t="s">
-        <v>780</v>
-      </c>
-      <c r="F62" t="s">
-        <v>781</v>
-      </c>
-      <c r="G62" t="s">
-        <v>782</v>
-      </c>
-      <c r="H62" t="s">
-        <v>783</v>
-      </c>
-      <c r="I62" t="s">
-        <v>784</v>
-      </c>
-      <c r="J62" t="s">
-        <v>785</v>
-      </c>
-      <c r="K62" t="s">
-        <v>786</v>
-      </c>
-      <c r="L62" t="s">
-        <v>787</v>
-      </c>
-      <c r="M62" t="s">
-        <v>788</v>
-      </c>
-      <c r="N62" t="s">
-        <v>789</v>
-      </c>
-      <c r="O62" t="s">
-        <v>790</v>
-      </c>
-      <c r="P62" t="s">
-        <v>791</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>792</v>
-      </c>
-      <c r="R62" t="s">
-        <v>793</v>
-      </c>
-      <c r="S62" t="s">
-        <v>794</v>
-      </c>
-      <c r="T62" t="s">
-        <v>795</v>
-      </c>
-      <c r="U62" t="s">
-        <v>796</v>
-      </c>
-      <c r="V62" t="s">
-        <v>797</v>
-      </c>
-      <c r="W62" t="s">
-        <v>798</v>
-      </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>799</v>
+        <v>778</v>
+      </c>
+      <c r="C63" t="s">
+        <v>779</v>
+      </c>
+      <c r="D63" t="s">
+        <v>780</v>
+      </c>
+      <c r="E63" t="s">
+        <v>781</v>
+      </c>
+      <c r="F63" t="s">
+        <v>782</v>
+      </c>
+      <c r="G63" t="s">
+        <v>783</v>
+      </c>
+      <c r="H63" t="s">
+        <v>784</v>
+      </c>
+      <c r="I63" t="s">
+        <v>89</v>
+      </c>
+      <c r="J63" t="s">
+        <v>88</v>
+      </c>
+      <c r="K63" t="s">
+        <v>785</v>
+      </c>
+      <c r="L63" t="s">
+        <v>786</v>
+      </c>
+      <c r="M63" t="s">
+        <v>787</v>
+      </c>
+      <c r="N63" t="s">
+        <v>788</v>
+      </c>
+      <c r="O63" t="s">
+        <v>360</v>
+      </c>
+      <c r="P63" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>789</v>
+      </c>
+      <c r="R63" t="s">
+        <v>85</v>
+      </c>
+      <c r="S63" t="s">
+        <v>790</v>
+      </c>
+      <c r="T63" t="s">
+        <v>791</v>
+      </c>
+      <c r="U63" t="s">
+        <v>785</v>
+      </c>
+      <c r="V63" t="s">
+        <v>792</v>
+      </c>
+      <c r="W63" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
@@ -7154,64 +7088,64 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
+        <v>794</v>
+      </c>
+      <c r="C64" t="s">
+        <v>795</v>
+      </c>
+      <c r="D64" t="s">
+        <v>796</v>
+      </c>
+      <c r="E64" t="s">
+        <v>797</v>
+      </c>
+      <c r="F64" t="s">
+        <v>798</v>
+      </c>
+      <c r="G64" t="s">
+        <v>799</v>
+      </c>
+      <c r="H64" t="s">
         <v>800</v>
       </c>
-      <c r="C64" t="s">
+      <c r="I64" t="s">
         <v>801</v>
       </c>
-      <c r="D64" t="s">
+      <c r="J64" t="s">
         <v>802</v>
       </c>
-      <c r="E64" t="s">
+      <c r="K64" t="s">
         <v>803</v>
       </c>
-      <c r="F64" t="s">
+      <c r="L64" t="s">
         <v>804</v>
       </c>
-      <c r="G64" t="s">
+      <c r="M64" t="s">
         <v>805</v>
       </c>
-      <c r="H64" t="s">
+      <c r="N64" t="s">
         <v>806</v>
       </c>
-      <c r="I64" t="s">
-        <v>89</v>
-      </c>
-      <c r="J64" t="s">
-        <v>88</v>
-      </c>
-      <c r="K64" t="s">
+      <c r="O64" t="s">
         <v>807</v>
       </c>
-      <c r="L64" t="s">
+      <c r="P64" t="s">
         <v>808</v>
       </c>
-      <c r="M64" t="s">
+      <c r="Q64" t="s">
         <v>809</v>
       </c>
-      <c r="N64" t="s">
+      <c r="R64" t="s">
         <v>810</v>
       </c>
-      <c r="O64" t="s">
-        <v>360</v>
-      </c>
-      <c r="P64" t="s">
-        <v>645</v>
-      </c>
-      <c r="Q64" t="s">
+      <c r="S64" t="s">
         <v>811</v>
       </c>
-      <c r="R64" t="s">
-        <v>85</v>
-      </c>
-      <c r="S64" t="s">
+      <c r="T64" t="s">
         <v>812</v>
       </c>
-      <c r="T64" t="s">
+      <c r="U64" t="s">
         <v>813</v>
-      </c>
-      <c r="U64" t="s">
-        <v>807</v>
       </c>
       <c r="V64" t="s">
         <v>814</v>
@@ -7228,139 +7162,73 @@
         <v>816</v>
       </c>
       <c r="C65" t="s">
+        <v>677</v>
+      </c>
+      <c r="D65" t="s">
         <v>817</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>818</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>819</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
+        <v>677</v>
+      </c>
+      <c r="H65" t="s">
+        <v>677</v>
+      </c>
+      <c r="I65" t="s">
+        <v>677</v>
+      </c>
+      <c r="J65" t="s">
+        <v>677</v>
+      </c>
+      <c r="K65" t="s">
+        <v>677</v>
+      </c>
+      <c r="L65" t="s">
+        <v>677</v>
+      </c>
+      <c r="M65" t="s">
+        <v>677</v>
+      </c>
+      <c r="N65" t="s">
+        <v>677</v>
+      </c>
+      <c r="O65" t="s">
+        <v>677</v>
+      </c>
+      <c r="P65" t="s">
+        <v>677</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>677</v>
+      </c>
+      <c r="R65" t="s">
         <v>820</v>
       </c>
-      <c r="G65" t="s">
-        <v>821</v>
-      </c>
-      <c r="H65" t="s">
-        <v>822</v>
-      </c>
-      <c r="I65" t="s">
-        <v>823</v>
-      </c>
-      <c r="J65" t="s">
-        <v>824</v>
-      </c>
-      <c r="K65" t="s">
-        <v>825</v>
-      </c>
-      <c r="L65" t="s">
-        <v>826</v>
-      </c>
-      <c r="M65" t="s">
-        <v>827</v>
-      </c>
-      <c r="N65" t="s">
-        <v>828</v>
-      </c>
-      <c r="O65" t="s">
-        <v>829</v>
-      </c>
-      <c r="P65" t="s">
-        <v>830</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>831</v>
-      </c>
-      <c r="R65" t="s">
-        <v>832</v>
-      </c>
       <c r="S65" t="s">
-        <v>833</v>
+        <v>677</v>
       </c>
       <c r="T65" t="s">
-        <v>834</v>
+        <v>677</v>
       </c>
       <c r="U65" t="s">
-        <v>835</v>
+        <v>677</v>
       </c>
       <c r="V65" t="s">
-        <v>836</v>
+        <v>677</v>
       </c>
       <c r="W65" t="s">
-        <v>837</v>
+        <v>677</v>
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" t="s">
-        <v>838</v>
-      </c>
-      <c r="C66" t="s">
-        <v>699</v>
-      </c>
-      <c r="D66" t="s">
-        <v>839</v>
-      </c>
-      <c r="E66" t="s">
-        <v>840</v>
-      </c>
-      <c r="F66" t="s">
-        <v>841</v>
-      </c>
-      <c r="G66" t="s">
-        <v>699</v>
-      </c>
-      <c r="H66" t="s">
-        <v>699</v>
-      </c>
-      <c r="I66" t="s">
-        <v>699</v>
-      </c>
-      <c r="J66" t="s">
-        <v>699</v>
-      </c>
-      <c r="K66" t="s">
-        <v>699</v>
-      </c>
-      <c r="L66" t="s">
-        <v>699</v>
-      </c>
-      <c r="M66" t="s">
-        <v>699</v>
-      </c>
-      <c r="N66" t="s">
-        <v>699</v>
-      </c>
-      <c r="O66" t="s">
-        <v>699</v>
-      </c>
-      <c r="P66" t="s">
-        <v>699</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>699</v>
-      </c>
-      <c r="R66" t="s">
-        <v>842</v>
-      </c>
-      <c r="S66" t="s">
-        <v>699</v>
-      </c>
-      <c r="T66" t="s">
-        <v>699</v>
-      </c>
-      <c r="U66" t="s">
-        <v>699</v>
-      </c>
-      <c r="V66" t="s">
-        <v>699</v>
-      </c>
-      <c r="W66" t="s">
-        <v>699</v>
-      </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
@@ -7377,43 +7245,43 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="C69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="D69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="E69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="F69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="G69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="H69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="I69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="J69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="K69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="L69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="M69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="N69" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.25">
@@ -7421,70 +7289,70 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>845</v>
+        <v>823</v>
       </c>
       <c r="C70" t="s">
-        <v>846</v>
+        <v>824</v>
       </c>
       <c r="D70" t="s">
-        <v>847</v>
+        <v>825</v>
       </c>
       <c r="E70" t="s">
-        <v>848</v>
+        <v>826</v>
       </c>
       <c r="F70" t="s">
-        <v>849</v>
+        <v>827</v>
       </c>
       <c r="G70" t="s">
-        <v>850</v>
+        <v>828</v>
       </c>
       <c r="H70" t="s">
-        <v>851</v>
+        <v>829</v>
       </c>
       <c r="I70" t="s">
-        <v>852</v>
+        <v>830</v>
       </c>
       <c r="J70" t="s">
-        <v>853</v>
+        <v>831</v>
       </c>
       <c r="K70" t="s">
-        <v>854</v>
+        <v>832</v>
       </c>
       <c r="L70" t="s">
-        <v>855</v>
+        <v>833</v>
       </c>
       <c r="M70" t="s">
-        <v>856</v>
+        <v>834</v>
       </c>
       <c r="N70" t="s">
-        <v>857</v>
+        <v>835</v>
       </c>
       <c r="O70" t="s">
-        <v>858</v>
+        <v>836</v>
       </c>
       <c r="P70" t="s">
-        <v>859</v>
+        <v>837</v>
       </c>
       <c r="Q70" t="s">
-        <v>860</v>
+        <v>838</v>
       </c>
       <c r="R70" t="s">
-        <v>861</v>
+        <v>839</v>
       </c>
       <c r="S70" t="s">
-        <v>862</v>
+        <v>840</v>
       </c>
       <c r="T70" t="s">
-        <v>863</v>
+        <v>841</v>
       </c>
       <c r="U70" t="s">
-        <v>864</v>
+        <v>842</v>
       </c>
       <c r="V70" t="s">
-        <v>865</v>
+        <v>843</v>
       </c>
       <c r="W70" t="s">
-        <v>866</v>
+        <v>844</v>
       </c>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.25">
@@ -7492,70 +7360,70 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>867</v>
+        <v>845</v>
       </c>
       <c r="C71" t="s">
-        <v>868</v>
+        <v>846</v>
       </c>
       <c r="D71" t="s">
-        <v>869</v>
+        <v>847</v>
       </c>
       <c r="E71" t="s">
-        <v>870</v>
+        <v>848</v>
       </c>
       <c r="F71" t="s">
-        <v>871</v>
+        <v>849</v>
       </c>
       <c r="G71" t="s">
-        <v>496</v>
+        <v>474</v>
       </c>
       <c r="H71" t="s">
-        <v>872</v>
+        <v>850</v>
       </c>
       <c r="I71" t="s">
-        <v>873</v>
+        <v>851</v>
       </c>
       <c r="J71" t="s">
-        <v>874</v>
+        <v>852</v>
       </c>
       <c r="K71" t="s">
         <v>83</v>
       </c>
       <c r="L71" t="s">
-        <v>875</v>
+        <v>853</v>
       </c>
       <c r="M71" t="s">
-        <v>876</v>
+        <v>854</v>
       </c>
       <c r="N71" t="s">
-        <v>877</v>
+        <v>855</v>
       </c>
       <c r="O71" t="s">
-        <v>878</v>
+        <v>856</v>
       </c>
       <c r="P71" t="s">
-        <v>879</v>
+        <v>857</v>
       </c>
       <c r="Q71" t="s">
-        <v>880</v>
+        <v>858</v>
       </c>
       <c r="R71" t="s">
-        <v>881</v>
+        <v>859</v>
       </c>
       <c r="S71" t="s">
-        <v>882</v>
+        <v>860</v>
       </c>
       <c r="T71" t="s">
-        <v>883</v>
+        <v>861</v>
       </c>
       <c r="U71" t="s">
         <v>93</v>
       </c>
       <c r="V71" t="s">
-        <v>882</v>
+        <v>860</v>
       </c>
       <c r="W71" t="s">
-        <v>884</v>
+        <v>862</v>
       </c>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.25">
@@ -7563,43 +7431,43 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>885</v>
+        <v>863</v>
       </c>
       <c r="C72" t="s">
-        <v>886</v>
+        <v>864</v>
       </c>
       <c r="D72" t="s">
-        <v>887</v>
+        <v>865</v>
       </c>
       <c r="E72" t="s">
-        <v>888</v>
+        <v>866</v>
       </c>
       <c r="F72" t="s">
-        <v>889</v>
+        <v>867</v>
       </c>
       <c r="G72" t="s">
-        <v>890</v>
+        <v>868</v>
       </c>
       <c r="H72" t="s">
-        <v>891</v>
+        <v>869</v>
       </c>
       <c r="I72" t="s">
-        <v>892</v>
+        <v>870</v>
       </c>
       <c r="J72" t="s">
-        <v>893</v>
+        <v>871</v>
       </c>
       <c r="K72" t="s">
-        <v>894</v>
+        <v>872</v>
       </c>
       <c r="L72" t="s">
-        <v>895</v>
+        <v>873</v>
       </c>
       <c r="M72" t="s">
-        <v>896</v>
+        <v>874</v>
       </c>
       <c r="N72" t="s">
-        <v>897</v>
+        <v>875</v>
       </c>
       <c r="O72" t="s">
         <v>329</v>
@@ -7608,25 +7476,25 @@
         <v>196</v>
       </c>
       <c r="Q72" t="s">
-        <v>898</v>
+        <v>876</v>
       </c>
       <c r="R72" t="s">
-        <v>899</v>
+        <v>877</v>
       </c>
       <c r="S72" t="s">
-        <v>900</v>
+        <v>878</v>
       </c>
       <c r="T72" t="s">
-        <v>901</v>
+        <v>879</v>
       </c>
       <c r="U72" t="s">
-        <v>902</v>
+        <v>880</v>
       </c>
       <c r="V72" t="s">
-        <v>486</v>
+        <v>464</v>
       </c>
       <c r="W72" t="s">
-        <v>903</v>
+        <v>881</v>
       </c>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.25">
@@ -7634,70 +7502,70 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>904</v>
+        <v>882</v>
       </c>
       <c r="C73" t="s">
-        <v>872</v>
+        <v>850</v>
       </c>
       <c r="D73" t="s">
-        <v>877</v>
+        <v>855</v>
       </c>
       <c r="E73" t="s">
-        <v>905</v>
+        <v>883</v>
       </c>
       <c r="F73" t="s">
-        <v>906</v>
+        <v>884</v>
       </c>
       <c r="G73" t="s">
-        <v>907</v>
+        <v>885</v>
       </c>
       <c r="H73" t="s">
-        <v>908</v>
+        <v>886</v>
       </c>
       <c r="I73" t="s">
-        <v>909</v>
+        <v>887</v>
       </c>
       <c r="J73" t="s">
-        <v>910</v>
+        <v>888</v>
       </c>
       <c r="K73" t="s">
-        <v>420</v>
+        <v>398</v>
       </c>
       <c r="L73" t="s">
-        <v>911</v>
+        <v>889</v>
       </c>
       <c r="M73" t="s">
-        <v>907</v>
+        <v>885</v>
       </c>
       <c r="N73" t="s">
-        <v>907</v>
+        <v>885</v>
       </c>
       <c r="O73" t="s">
-        <v>912</v>
+        <v>890</v>
       </c>
       <c r="P73" t="s">
-        <v>913</v>
+        <v>891</v>
       </c>
       <c r="Q73" t="s">
-        <v>914</v>
+        <v>892</v>
       </c>
       <c r="R73" t="s">
-        <v>512</v>
+        <v>490</v>
       </c>
       <c r="S73" t="s">
-        <v>877</v>
+        <v>855</v>
       </c>
       <c r="T73" t="s">
-        <v>915</v>
+        <v>893</v>
       </c>
       <c r="U73" t="s">
-        <v>496</v>
+        <v>474</v>
       </c>
       <c r="V73" t="s">
-        <v>916</v>
+        <v>894</v>
       </c>
       <c r="W73" t="s">
-        <v>917</v>
+        <v>895</v>
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.25">
@@ -7705,43 +7573,43 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="C74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="D74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="E74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="F74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="G74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="H74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="I74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="J74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="K74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="L74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="M74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="N74" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.25">
@@ -7749,70 +7617,70 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>919</v>
+        <v>897</v>
       </c>
       <c r="C75" t="s">
-        <v>920</v>
+        <v>898</v>
       </c>
       <c r="D75" t="s">
-        <v>921</v>
+        <v>899</v>
       </c>
       <c r="E75" t="s">
-        <v>922</v>
+        <v>900</v>
       </c>
       <c r="F75" t="s">
-        <v>923</v>
+        <v>901</v>
       </c>
       <c r="G75" t="s">
-        <v>924</v>
+        <v>902</v>
       </c>
       <c r="H75" t="s">
-        <v>925</v>
+        <v>903</v>
       </c>
       <c r="I75" t="s">
-        <v>926</v>
+        <v>904</v>
       </c>
       <c r="J75" t="s">
-        <v>927</v>
+        <v>905</v>
       </c>
       <c r="K75" t="s">
-        <v>928</v>
+        <v>906</v>
       </c>
       <c r="L75" t="s">
-        <v>929</v>
+        <v>907</v>
       </c>
       <c r="M75" t="s">
-        <v>930</v>
+        <v>908</v>
       </c>
       <c r="N75" t="s">
-        <v>931</v>
+        <v>909</v>
       </c>
       <c r="O75" t="s">
-        <v>932</v>
+        <v>910</v>
       </c>
       <c r="P75" t="s">
-        <v>933</v>
+        <v>911</v>
       </c>
       <c r="Q75" t="s">
-        <v>934</v>
+        <v>912</v>
       </c>
       <c r="R75" t="s">
-        <v>935</v>
+        <v>913</v>
       </c>
       <c r="S75" t="s">
-        <v>936</v>
+        <v>914</v>
       </c>
       <c r="T75" t="s">
-        <v>937</v>
+        <v>915</v>
       </c>
       <c r="U75" t="s">
-        <v>938</v>
+        <v>916</v>
       </c>
       <c r="V75" t="s">
-        <v>939</v>
+        <v>917</v>
       </c>
       <c r="W75" t="s">
-        <v>940</v>
+        <v>918</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.25">
@@ -7820,16 +7688,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>941</v>
+        <v>919</v>
       </c>
       <c r="C76" t="s">
-        <v>942</v>
+        <v>920</v>
       </c>
       <c r="D76" t="s">
         <v>42</v>
       </c>
       <c r="E76" t="s">
-        <v>943</v>
+        <v>921</v>
       </c>
       <c r="F76" t="s">
         <v>143</v>
@@ -7838,16 +7706,16 @@
         <v>124</v>
       </c>
       <c r="H76" t="s">
-        <v>944</v>
+        <v>922</v>
       </c>
       <c r="I76" t="s">
-        <v>945</v>
+        <v>923</v>
       </c>
       <c r="J76" t="s">
-        <v>491</v>
+        <v>469</v>
       </c>
       <c r="K76" t="s">
-        <v>946</v>
+        <v>924</v>
       </c>
       <c r="L76" t="s">
         <v>122</v>
@@ -7856,19 +7724,19 @@
         <v>139</v>
       </c>
       <c r="N76" t="s">
-        <v>947</v>
+        <v>925</v>
       </c>
       <c r="O76" t="s">
-        <v>948</v>
+        <v>926</v>
       </c>
       <c r="P76" t="s">
-        <v>949</v>
+        <v>927</v>
       </c>
       <c r="Q76" t="s">
-        <v>950</v>
+        <v>928</v>
       </c>
       <c r="R76" t="s">
-        <v>486</v>
+        <v>464</v>
       </c>
       <c r="S76" t="s">
         <v>120</v>
@@ -7880,7 +7748,7 @@
         <v>366</v>
       </c>
       <c r="V76" t="s">
-        <v>898</v>
+        <v>876</v>
       </c>
       <c r="W76" t="s">
         <v>45</v>
@@ -7891,7 +7759,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>951</v>
+        <v>929</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
@@ -7899,19 +7767,19 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>952</v>
+        <v>930</v>
       </c>
       <c r="C78" t="s">
         <v>197</v>
       </c>
       <c r="D78" t="s">
-        <v>953</v>
+        <v>931</v>
       </c>
       <c r="E78" t="s">
         <v>330</v>
       </c>
       <c r="F78" t="s">
-        <v>489</v>
+        <v>467</v>
       </c>
       <c r="G78" t="s">
         <v>69</v>
@@ -7920,22 +7788,22 @@
         <v>138</v>
       </c>
       <c r="I78" t="s">
-        <v>946</v>
+        <v>924</v>
       </c>
       <c r="J78" t="s">
-        <v>954</v>
+        <v>932</v>
       </c>
       <c r="K78" t="s">
-        <v>954</v>
+        <v>932</v>
       </c>
       <c r="L78" t="s">
-        <v>531</v>
+        <v>509</v>
       </c>
       <c r="M78" t="s">
-        <v>485</v>
+        <v>463</v>
       </c>
       <c r="N78" t="s">
-        <v>955</v>
+        <v>933</v>
       </c>
       <c r="O78" t="s">
         <v>119</v>
@@ -7944,22 +7812,22 @@
         <v>67</v>
       </c>
       <c r="Q78" t="s">
-        <v>956</v>
+        <v>934</v>
       </c>
       <c r="R78" t="s">
         <v>65</v>
       </c>
       <c r="S78" t="s">
-        <v>957</v>
+        <v>935</v>
       </c>
       <c r="T78" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="U78" t="s">
         <v>354</v>
       </c>
       <c r="V78" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="W78" t="s">
         <v>117</v>
@@ -7968,40 +7836,40 @@
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" t="s">
-        <v>960</v>
+        <v>938</v>
       </c>
       <c r="C79" t="s">
-        <v>961</v>
+        <v>939</v>
       </c>
       <c r="D79" t="s">
-        <v>962</v>
+        <v>940</v>
       </c>
       <c r="E79" t="s">
-        <v>494</v>
+        <v>472</v>
       </c>
       <c r="F79" t="s">
-        <v>963</v>
+        <v>941</v>
       </c>
       <c r="G79" t="s">
-        <v>491</v>
+        <v>469</v>
       </c>
       <c r="H79" t="s">
-        <v>964</v>
+        <v>942</v>
       </c>
       <c r="I79" t="s">
         <v>156</v>
       </c>
       <c r="J79" t="s">
-        <v>490</v>
+        <v>468</v>
       </c>
       <c r="K79" t="s">
-        <v>965</v>
+        <v>943</v>
       </c>
       <c r="L79" t="s">
-        <v>946</v>
+        <v>924</v>
       </c>
       <c r="M79" t="s">
-        <v>843</v>
+        <v>821</v>
       </c>
       <c r="N79" t="s">
         <v>155</v>
@@ -8010,19 +7878,19 @@
         <v>320</v>
       </c>
       <c r="P79" t="s">
-        <v>966</v>
+        <v>944</v>
       </c>
       <c r="Q79" t="s">
         <v>71</v>
       </c>
       <c r="R79" t="s">
-        <v>491</v>
+        <v>469</v>
       </c>
       <c r="S79" t="s">
-        <v>669</v>
+        <v>647</v>
       </c>
       <c r="T79" t="s">
-        <v>490</v>
+        <v>468</v>
       </c>
       <c r="U79" t="s">
         <v>365</v>
@@ -8037,70 +7905,70 @@
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="C80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="D80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="E80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="F80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="G80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="H80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="I80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="J80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="K80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="L80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="M80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="N80" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="O80" t="s">
-        <v>968</v>
+        <v>946</v>
       </c>
       <c r="P80" t="s">
-        <v>968</v>
+        <v>946</v>
       </c>
       <c r="Q80" t="s">
-        <v>968</v>
+        <v>946</v>
       </c>
       <c r="R80" t="s">
-        <v>968</v>
+        <v>946</v>
       </c>
       <c r="S80" t="s">
-        <v>968</v>
+        <v>946</v>
       </c>
       <c r="T80" t="s">
-        <v>968</v>
+        <v>946</v>
       </c>
       <c r="U80" t="s">
-        <v>968</v>
+        <v>946</v>
       </c>
       <c r="V80" t="s">
-        <v>968</v>
+        <v>946</v>
       </c>
       <c r="W80" t="s">
-        <v>968</v>
+        <v>946</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>